<commit_message>
Complete output vs outputInfo
</commit_message>
<xml_diff>
--- a/Bang danh sach cong việc.xlsx
+++ b/Bang danh sach cong việc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Danh sách module</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>method login chua lam</t>
+  </si>
+  <si>
+    <t>delete vs update ko làm vì cảm thấy ko cần</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,8 +467,8 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="43" customWidth="1"/>
     <col min="10" max="10" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -629,8 +632,17 @@
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
       <c r="E11" s="3"/>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -639,8 +651,14 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
       <c r="E12" s="3"/>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -649,6 +667,7 @@
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
     </row>

</xml_diff>